<commit_message>
second commit: using RE Framework
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinesh\Documents\UiPath\Robot-5_Recipe_Scraping_Process_RE\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -123,11 +122,17 @@
   <si>
     <t>OrchestratorAssetFolder</t>
   </si>
+  <si>
+    <t>SiteURL</t>
+  </si>
+  <si>
+    <t>https://www.taste.com.au/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -496,11 +501,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -569,7 +574,14 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1569,7 +1581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2679,10 +2691,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>